<commit_message>
Function added to add all papers from TSPapers.csv into Pubscreen
</commit_message>
<xml_diff>
--- a/TSPapers.xlsx
+++ b/TSPapers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Jiang\Documents\GitHub\CBAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97801B90-9D74-48E9-BA67-6E4DC6C053DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6438F0-2A69-42FD-B3AB-335AD5D9AC2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4724" uniqueCount="3275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4723" uniqueCount="3274">
   <si>
     <t>Year</t>
   </si>
@@ -10147,9 +10147,6 @@
   </si>
   <si>
     <t>10.1016/j.celrep.2021.108741</t>
-  </si>
-  <si>
-    <t>10.1101/lm.987808</t>
   </si>
 </sst>
 </file>
@@ -10480,10 +10477,10 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14290,7 +14287,7 @@
   <dimension ref="A1:BI415"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -14339,12 +14336,8 @@
         <v>9</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="55" t="s">
-        <v>3274</v>
-      </c>
-      <c r="G2" s="55">
-        <v>18612068</v>
-      </c>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
@@ -22473,11 +22466,9 @@
     <hyperlink ref="F332" r:id="rId1" display="https://doi.org/10.1080/1028415x.2020.1809879" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="G332" r:id="rId2" display="http://pubmed.ncbi.nlm.nih.gov/32840166/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="F354" r:id="rId3" tooltip="Persistent link using digital object identifier" display="https://doi-org.proxy1.lib.uwo.ca/10.1016/j.neulet.2020.135378" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F2" r:id="rId4" display="https://dx.doi.org/10.1101%2Flm.987808" xr:uid="{26EA3CBB-B97D-4132-A604-0F452D808560}"/>
-    <hyperlink ref="G2" r:id="rId5" display="https://www.ncbi.nlm.nih.gov/pubmed/18612068" xr:uid="{4840CAC2-1A51-45EB-944A-0411FDE1D1F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -38335,10 +38326,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>2904</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">

</xml_diff>